<commit_message>
Revert "Asignado nombre al"
This reverts commit bede35ec0bd49fa6c3fe4b1c0bbacf4792d67a81.
</commit_message>
<xml_diff>
--- a/08/Articulos.xlsx
+++ b/08/Articulos.xlsx
@@ -14,9 +14,6 @@
   <sheets>
     <sheet name="Artículos" sheetId="2" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="TablaArticulos">Artículos!$A$2:$C$8</definedName>
-  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -405,7 +402,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Asignado nombre al área de datos de la hoja de artículos
</commit_message>
<xml_diff>
--- a/08/Articulos.xlsx
+++ b/08/Articulos.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Artículos" sheetId="2" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="TablaArticulos">Artículos!$A$2:$C$8</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -402,7 +405,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Asignados nombres a las columnas de datos
</commit_message>
<xml_diff>
--- a/08/Articulos.xlsx
+++ b/08/Articulos.xlsx
@@ -15,6 +15,8 @@
     <sheet name="Artículos" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="Descripcion">Artículos!$B$1</definedName>
+    <definedName name="Precio">Artículos!$C$1</definedName>
     <definedName name="TablaArticulos">Artículos!$A$2:$C$8</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -27,15 +29,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Código</t>
   </si>
   <si>
     <t>Descripción</t>
-  </si>
-  <si>
-    <t>Articulos</t>
   </si>
   <si>
     <t>Precio</t>
@@ -404,9 +403,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C8"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -414,8 +411,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
         <v>2</v>
+      </c>
+      <c r="C1">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -426,7 +429,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -434,7 +437,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3">
         <v>22.9</v>
@@ -445,7 +448,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4">
         <v>21</v>
@@ -456,7 +459,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <v>21</v>
@@ -467,7 +470,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <v>12</v>
@@ -478,7 +481,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7">
         <v>7</v>
@@ -489,7 +492,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8">
         <v>21</v>

</xml_diff>